<commit_message>
sửa nội dung trong luận thiên mã
</commit_message>
<xml_diff>
--- a/LoiKhuyen.xlsx
+++ b/LoiKhuyen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B758F9C6-66E2-4248-81BE-A5D2C7B3E67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00313E7-F2E3-4492-82E8-B819F2FA7803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Can sinh Chi</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Bạn phải lao tâm, vất vả lo nghĩ về những thay đổi, bạn rất năng động và hay phải đi xa rất nhiều. Hãy cố gắng bình tĩnh giữ gìn thể-trí để gặt hái nhiều điều tốt đẹp.</t>
+  </si>
+  <si>
+    <t>Bạn đi ra ngoài hay gặp điều kém may mắn nhưng không vì thế mà không cố gắng, chỉ có năng động tích cực mới giúp bạn có nhiều cơ hội hơn.</t>
+  </si>
+  <si>
+    <t>Bạn ra ngoài luôn gặp may mắn, tiến hành công việc dễ xứng ý toại lòng. Nhưng không vì thế mà bất cẩn trong đi lại hay công việc.</t>
+  </si>
+  <si>
+    <t>Bạn có thể gặp khó khăn khi đi lại hoặc trong công việc nhưng hầu hết bạn đều có thể xử lý tốt mọi vấn đề phát sinh.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,15 +549,24 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add file luận giải
</commit_message>
<xml_diff>
--- a/LoiKhuyen.xlsx
+++ b/LoiKhuyen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00313E7-F2E3-4492-82E8-B819F2FA7803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA66D8C4-45AC-4083-93CD-4F96CEF16A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Can sinh Chi</t>
   </si>
@@ -81,18 +81,6 @@
     <t>Tang Tuế Điếu</t>
   </si>
   <si>
-    <t>Bạn là người thông minh, biết cách ứng xử phù hợp và nên giữ đức tính nhu thuận làm kim chỉ nam cuộc đời để gặp nhiều may mắn.</t>
-  </si>
-  <si>
-    <t>Bạn là người sinh đúng thời, cuộc sống gặp nhiều thuận lợi và may mắn. Tránh đề cao cái tôi thái quá để lỡ mất nhiều cơ hội.</t>
-  </si>
-  <si>
-    <t>Bạn là người thông minh tuy nhiên luôn đề cao cái tôi và luôn cố gắng thắng trong mọi cuộc chơi nên dễ gây ra nhiều thị phi. Bạn nên đề cao sự tử tế và nhu thuận hơn để gặp nhiều sự hỗ trợ từ mọi người.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bạn là người năng động luôn cố gắng xoay sở để có thể cải thiện vị thế bản thân, tuy nhiên cần cẩn trọng việc đi lại, giữ bình tĩnh tránh mất </t>
-  </si>
-  <si>
     <t>Ngũ hành bản Mệnh sinh Ngũ hành Thiên Mã</t>
   </si>
   <si>
@@ -121,6 +109,21 @@
   </si>
   <si>
     <t>Bạn có thể gặp khó khăn khi đi lại hoặc trong công việc nhưng hầu hết bạn đều có thể xử lý tốt mọi vấn đề phát sinh.</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh tuy nhiên luôn đề cao cái tôi và luôn cố gắng thắng trong mọi cuộc chơi nên dễ gây ra nhiều thị phi. Bạn nên đề cao sự tử tế và nhu thuận hơn thì sẽ gặp nhiều sự hỗ trợ từ mọi người.</t>
+  </si>
+  <si>
+    <t>Bạn là người năng động luôn cố gắng xoay sở để có thể cải thiện vị thế bản thân, tuy nhiên cần cẩn trọng việc đi lại, giữ hòa khí với mọi người.</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh, biết cách ứng xử phù hợp và nên giữ đức tính nhu thuận làm kim chỉ nam cuộc đời để gặp nhiều may mắn. Thuận thiên vô chiến tự nhiên thành.</t>
+  </si>
+  <si>
+    <t>Đặc biệt điều tiên quyét là bạn phải biết chọn bạn mà chơi chọn thầy mà theo thì bạn mới gặt được thành quả tốt đẹp.</t>
+  </si>
+  <si>
+    <t>Bạn sinh ra gặp rất nhiều sóng gió cuộc đời nhưng đừng nản chí và bỏ cuộc vì đến khi vào đại vận bạn sẽ đủ chín chắn, trưởng thành do tích lũy trước đó. Bạn sẽ được hưởng trọn vẹn thành quả của sự cố gắng, cuộc sống gắn liền phần nhiều đến tín ngưỡng và tôn giáo. Bạn hãy cố gắng trau dồi kinh nghiệm, kiến thức và trải nghiệm.</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +452,7 @@
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -465,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -473,7 +476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -481,7 +484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -489,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -497,7 +500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -505,76 +508,79 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B16" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sửa lại nội dung luận trong file excel
</commit_message>
<xml_diff>
--- a/LoiKhuyen.xlsx
+++ b/LoiKhuyen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA66D8C4-45AC-4083-93CD-4F96CEF16A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82266C56-E968-4CD4-9D46-7B447EDDAE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>Bạn có Phúc đức quá lớn, tiềm tàng hơn người. Hãy làm việc tốt để tích thêm phước báu.</t>
   </si>
   <si>
-    <t>Bạn có thể gặp nhiều khó khăn trong cuộc sống. Tuy nhiên có công mài sắt có ngày nên kim.</t>
-  </si>
-  <si>
-    <t>Bạn gặp nhiều may mắn hơn thực lực bản thân. Hãy cố gắng trau dồi năng lực để càng gặp nhiều điều toại nguyện hơn.</t>
-  </si>
-  <si>
     <t>Cuộc đời của bạn nhiều điều không toại lòng. Hãy kiên định và cố gắng sẽ có quả ngọt, cẩn thận trong cả lúc thuận lợi nhất.</t>
   </si>
   <si>
@@ -123,7 +117,13 @@
     <t>Đặc biệt điều tiên quyét là bạn phải biết chọn bạn mà chơi chọn thầy mà theo thì bạn mới gặt được thành quả tốt đẹp.</t>
   </si>
   <si>
-    <t>Bạn sinh ra gặp rất nhiều sóng gió cuộc đời nhưng đừng nản chí và bỏ cuộc vì đến khi vào đại vận bạn sẽ đủ chín chắn, trưởng thành do tích lũy trước đó. Bạn sẽ được hưởng trọn vẹn thành quả của sự cố gắng, cuộc sống gắn liền phần nhiều đến tín ngưỡng và tôn giáo. Bạn hãy cố gắng trau dồi kinh nghiệm, kiến thức và trải nghiệm.</t>
+    <t>Bạn là người giàu nghị lực và có thể gặp nhiều khó khăn trong cuộc sống. Tuy nhiên "lửa thử vàng, gian nan thử sức", hãy cố gắng trở thành hòn ngọc quý.</t>
+  </si>
+  <si>
+    <t>Bạn gặp nhiều may mắn hơn thực lực bản thân. Hãy cố gắng trau dồi năng lực của bản thân để càng gặp nhiều điều toại nguyện hơn.</t>
+  </si>
+  <si>
+    <t>Bạn sinh ra gặp rất nhiều sóng gió cuộc đời nhưng đừng nản chí và bỏ cuộc vì đến khi vào đại vận trung niên bạn sẽ được hưởng trọn vẹn thành quả của sự cố gắng do quá trình tích lũy trước đó, cuộc sống gắn liền phần nhiều đến tín ngưỡng và tôn giáo. Bạn hãy cố gắng trau dồi kinh nghiệm, kiến thức và trải nghiệm.</t>
   </si>
 </sst>
 </file>
@@ -139,12 +139,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,8 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +451,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +460,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -461,19 +468,19 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,23 +501,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -518,69 +525,69 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>